<commit_message>
update as of 12 8 2021
</commit_message>
<xml_diff>
--- a/RAnalysis/Data/Seawater_chemistry/Water_Chemistry_Scallops_2021_RAWUPLOAD.xlsx
+++ b/RAnalysis/Data/Seawater_chemistry/Water_Chemistry_Scallops_2021_RAWUPLOAD.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samjg\Documents\Github_repositories\Airradians_OA\RAnalysis\Data\Seawater_chemistry\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samuel.gurr\Documents\Github_repositories\Airradians_OA-foodsupply\RAnalysis\Data\Seawater_chemistry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7AC12AFC-93FC-4F56-8C73-CC5E727003AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="-110" windowWidth="18490" windowHeight="12220"/>
+    <workbookView xWindow="816" yWindow="-108" windowWidth="18492" windowHeight="12216"/>
   </bookViews>
   <sheets>
     <sheet name="Water_Chemistry_Scallops_2021_R" sheetId="1" r:id="rId1"/>
@@ -1056,16 +1055,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X282"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="B89" sqref="B89"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="Q132" sqref="Q132"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.81640625" customWidth="1"/>
+    <col min="1" max="1" width="23.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1136,7 +1135,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>44403</v>
       </c>
@@ -1204,7 +1203,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>44403</v>
       </c>
@@ -1272,7 +1271,7 @@
         <v>1.83</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>44403</v>
       </c>
@@ -1340,7 +1339,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>44403</v>
       </c>
@@ -1408,7 +1407,7 @@
         <v>1.87</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>44403</v>
       </c>
@@ -1476,7 +1475,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>44403</v>
       </c>
@@ -1544,7 +1543,7 @@
         <v>1.23</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>44403</v>
       </c>
@@ -1612,7 +1611,7 @@
         <v>1.37</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>44403</v>
       </c>
@@ -1680,7 +1679,7 @@
         <v>1.26</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>44403</v>
       </c>
@@ -1748,7 +1747,7 @@
         <v>1.41</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>44403</v>
       </c>
@@ -1816,7 +1815,7 @@
         <v>1.27</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>44403</v>
       </c>
@@ -1884,7 +1883,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>44403</v>
       </c>
@@ -1952,7 +1951,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>44403</v>
       </c>
@@ -2020,7 +2019,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>44403</v>
       </c>
@@ -2088,7 +2087,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>44403</v>
       </c>
@@ -2156,7 +2155,7 @@
         <v>0.63</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>44405</v>
       </c>
@@ -2224,7 +2223,7 @@
         <v>1.83</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>44405</v>
       </c>
@@ -2292,7 +2291,7 @@
         <v>1.84</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>44405</v>
       </c>
@@ -2360,7 +2359,7 @@
         <v>1.87</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>44405</v>
       </c>
@@ -2428,7 +2427,7 @@
         <v>1.89</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>44405</v>
       </c>
@@ -2496,7 +2495,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>44405</v>
       </c>
@@ -2564,7 +2563,7 @@
         <v>1.26</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>44405</v>
       </c>
@@ -2632,7 +2631,7 @@
         <v>1.18</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>44405</v>
       </c>
@@ -2700,7 +2699,7 @@
         <v>1.21</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>44405</v>
       </c>
@@ -2768,7 +2767,7 @@
         <v>1.22</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>44405</v>
       </c>
@@ -2836,7 +2835,7 @@
         <v>1.26</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>44405</v>
       </c>
@@ -2904,7 +2903,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>44405</v>
       </c>
@@ -2972,7 +2971,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>44405</v>
       </c>
@@ -3040,7 +3039,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>44405</v>
       </c>
@@ -3108,7 +3107,7 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>44405</v>
       </c>
@@ -3176,7 +3175,7 @@
         <v>0.63</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>44407</v>
       </c>
@@ -3244,7 +3243,7 @@
         <v>1.98</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>44407</v>
       </c>
@@ -3312,7 +3311,7 @@
         <v>1.99</v>
       </c>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>44407</v>
       </c>
@@ -3380,7 +3379,7 @@
         <v>1.98</v>
       </c>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>44407</v>
       </c>
@@ -3448,7 +3447,7 @@
         <v>1.95</v>
       </c>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>44407</v>
       </c>
@@ -3516,7 +3515,7 @@
         <v>1.78</v>
       </c>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>44407</v>
       </c>
@@ -3584,7 +3583,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>44407</v>
       </c>
@@ -3652,7 +3651,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>44407</v>
       </c>
@@ -3720,7 +3719,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>44407</v>
       </c>
@@ -3788,7 +3787,7 @@
         <v>1.26</v>
       </c>
     </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>44407</v>
       </c>
@@ -3856,7 +3855,7 @@
         <v>1.29</v>
       </c>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>44407</v>
       </c>
@@ -3924,7 +3923,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>44407</v>
       </c>
@@ -3992,7 +3991,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>44407</v>
       </c>
@@ -4060,7 +4059,7 @@
         <v>0.69</v>
       </c>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>44407</v>
       </c>
@@ -4128,7 +4127,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>44407</v>
       </c>
@@ -4196,7 +4195,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>44411</v>
       </c>
@@ -4264,7 +4263,7 @@
         <v>1.96</v>
       </c>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>44411</v>
       </c>
@@ -4332,7 +4331,7 @@
         <v>1.95</v>
       </c>
     </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>44411</v>
       </c>
@@ -4400,7 +4399,7 @@
         <v>1.96</v>
       </c>
     </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>44411</v>
       </c>
@@ -4468,7 +4467,7 @@
         <v>1.96</v>
       </c>
     </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>44411</v>
       </c>
@@ -4536,7 +4535,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>44411</v>
       </c>
@@ -4604,7 +4603,7 @@
         <v>1.26</v>
       </c>
     </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>44411</v>
       </c>
@@ -4672,7 +4671,7 @@
         <v>1.22</v>
       </c>
     </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>44411</v>
       </c>
@@ -4740,7 +4739,7 @@
         <v>1.23</v>
       </c>
     </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>44411</v>
       </c>
@@ -4808,7 +4807,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>44411</v>
       </c>
@@ -4876,7 +4875,7 @@
         <v>1.27</v>
       </c>
     </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>44411</v>
       </c>
@@ -4944,7 +4943,7 @@
         <v>0.69</v>
       </c>
     </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>44411</v>
       </c>
@@ -5012,7 +5011,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>44411</v>
       </c>
@@ -5080,7 +5079,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="60" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>44411</v>
       </c>
@@ -5148,7 +5147,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>44411</v>
       </c>
@@ -5216,7 +5215,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>44413</v>
       </c>
@@ -5284,7 +5283,7 @@
         <v>2.02</v>
       </c>
     </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>44413</v>
       </c>
@@ -5352,7 +5351,7 @@
         <v>1.98</v>
       </c>
     </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>44413</v>
       </c>
@@ -5420,7 +5419,7 @@
         <v>1.97</v>
       </c>
     </row>
-    <row r="65" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>44413</v>
       </c>
@@ -5488,7 +5487,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>44413</v>
       </c>
@@ -5556,7 +5555,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="67" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>44413</v>
       </c>
@@ -5624,7 +5623,7 @@
         <v>1.24</v>
       </c>
     </row>
-    <row r="68" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>44413</v>
       </c>
@@ -5692,7 +5691,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="69" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>44413</v>
       </c>
@@ -5760,7 +5759,7 @@
         <v>1.24</v>
       </c>
     </row>
-    <row r="70" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>44413</v>
       </c>
@@ -5828,7 +5827,7 @@
         <v>1.28</v>
       </c>
     </row>
-    <row r="71" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>44413</v>
       </c>
@@ -5896,7 +5895,7 @@
         <v>1.26</v>
       </c>
     </row>
-    <row r="72" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>44413</v>
       </c>
@@ -5964,7 +5963,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="73" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>44413</v>
       </c>
@@ -6032,7 +6031,7 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="74" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>44413</v>
       </c>
@@ -6100,7 +6099,7 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="75" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>44413</v>
       </c>
@@ -6168,7 +6167,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="76" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>44413</v>
       </c>
@@ -6236,7 +6235,7 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="77" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>44417</v>
       </c>
@@ -6304,7 +6303,7 @@
         <v>1.94</v>
       </c>
     </row>
-    <row r="78" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>44417</v>
       </c>
@@ -6372,7 +6371,7 @@
         <v>1.84</v>
       </c>
     </row>
-    <row r="79" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>44417</v>
       </c>
@@ -6440,7 +6439,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="80" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>44417</v>
       </c>
@@ -6508,7 +6507,7 @@
         <v>1.82</v>
       </c>
     </row>
-    <row r="81" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>44417</v>
       </c>
@@ -6576,7 +6575,7 @@
         <v>1.69</v>
       </c>
     </row>
-    <row r="82" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>44417</v>
       </c>
@@ -6644,7 +6643,7 @@
         <v>1.23</v>
       </c>
     </row>
-    <row r="83" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>44417</v>
       </c>
@@ -6712,7 +6711,7 @@
         <v>1.22</v>
       </c>
     </row>
-    <row r="84" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>44417</v>
       </c>
@@ -6780,7 +6779,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="85" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>44417</v>
       </c>
@@ -6848,7 +6847,7 @@
         <v>1.28</v>
       </c>
     </row>
-    <row r="86" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>44417</v>
       </c>
@@ -6916,7 +6915,7 @@
         <v>1.31</v>
       </c>
     </row>
-    <row r="87" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>44417</v>
       </c>
@@ -6984,7 +6983,7 @@
         <v>0.69</v>
       </c>
     </row>
-    <row r="88" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>44417</v>
       </c>
@@ -7052,7 +7051,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="89" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>44417</v>
       </c>
@@ -7120,7 +7119,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="90" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>44417</v>
       </c>
@@ -7188,7 +7187,7 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="91" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>44417</v>
       </c>
@@ -7256,7 +7255,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="92" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>27</v>
       </c>
@@ -7300,7 +7299,7 @@
         <v>7.83</v>
       </c>
     </row>
-    <row r="93" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>29</v>
       </c>
@@ -7344,7 +7343,7 @@
         <v>7.6059999999999999</v>
       </c>
     </row>
-    <row r="94" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>44427</v>
       </c>
@@ -7415,7 +7414,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="95" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>44427</v>
       </c>
@@ -7486,7 +7485,7 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="96" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>44427</v>
       </c>
@@ -7557,7 +7556,7 @@
         <v>1.48</v>
       </c>
     </row>
-    <row r="97" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>44427</v>
       </c>
@@ -7628,7 +7627,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="98" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>44427</v>
       </c>
@@ -7699,7 +7698,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="99" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>44427</v>
       </c>
@@ -7770,7 +7769,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="100" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>44427</v>
       </c>
@@ -7841,7 +7840,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="101" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>44427</v>
       </c>
@@ -7912,7 +7911,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="102" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>44427</v>
       </c>
@@ -7983,7 +7982,7 @@
         <v>1.04</v>
       </c>
     </row>
-    <row r="103" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>44427</v>
       </c>
@@ -8054,7 +8053,7 @@
         <v>1.04</v>
       </c>
     </row>
-    <row r="104" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>44427</v>
       </c>
@@ -8125,7 +8124,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="105" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>44427</v>
       </c>
@@ -8196,7 +8195,7 @@
         <v>1.08</v>
       </c>
     </row>
-    <row r="106" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>44440</v>
       </c>
@@ -8267,7 +8266,7 @@
         <v>1.29</v>
       </c>
     </row>
-    <row r="107" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>44440</v>
       </c>
@@ -8338,7 +8337,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="108" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>44440</v>
       </c>
@@ -8409,7 +8408,7 @@
         <v>1.27</v>
       </c>
     </row>
-    <row r="109" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>44440</v>
       </c>
@@ -8480,7 +8479,7 @@
         <v>1.26</v>
       </c>
     </row>
-    <row r="110" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>44440</v>
       </c>
@@ -8551,7 +8550,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="111" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>44440</v>
       </c>
@@ -8622,7 +8621,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="112" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>44440</v>
       </c>
@@ -8693,7 +8692,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="113" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>44440</v>
       </c>
@@ -8764,7 +8763,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="114" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>44440</v>
       </c>
@@ -8835,7 +8834,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="115" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <v>44440</v>
       </c>
@@ -8906,7 +8905,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="116" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
         <v>44446</v>
       </c>
@@ -8977,7 +8976,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="117" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>44446</v>
       </c>
@@ -9048,7 +9047,7 @@
         <v>1.24</v>
       </c>
     </row>
-    <row r="118" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <v>44446</v>
       </c>
@@ -9119,7 +9118,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="119" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>44446</v>
       </c>
@@ -9190,7 +9189,7 @@
         <v>1.21</v>
       </c>
     </row>
-    <row r="120" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <v>44446</v>
       </c>
@@ -9261,7 +9260,7 @@
         <v>0.84</v>
       </c>
     </row>
-    <row r="121" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>44446</v>
       </c>
@@ -9332,7 +9331,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="122" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <v>44446</v>
       </c>
@@ -9403,7 +9402,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="123" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>44446</v>
       </c>
@@ -9474,7 +9473,7 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="124" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>44446</v>
       </c>
@@ -9545,7 +9544,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="125" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
         <v>44446</v>
       </c>
@@ -9616,7 +9615,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="126" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
         <v>44448</v>
       </c>
@@ -9687,7 +9686,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="127" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
         <v>44448</v>
       </c>
@@ -9758,7 +9757,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="128" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A128" s="1">
         <v>44448</v>
       </c>
@@ -9829,7 +9828,7 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="129" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A129" s="1">
         <v>44448</v>
       </c>
@@ -9900,7 +9899,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="130" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A130" s="1">
         <v>44448</v>
       </c>
@@ -9938,7 +9937,7 @@
         <v>1</v>
       </c>
       <c r="N130">
-        <v>921.9</v>
+        <v>1921.9</v>
       </c>
       <c r="O130">
         <v>1951.21</v>
@@ -9971,7 +9970,7 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="131" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A131" s="1">
         <v>44448</v>
       </c>
@@ -10042,7 +10041,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="132" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A132" s="1">
         <v>44448</v>
       </c>
@@ -10113,7 +10112,7 @@
         <v>1.54</v>
       </c>
     </row>
-    <row r="133" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A133" s="1">
         <v>44448</v>
       </c>
@@ -10184,7 +10183,7 @@
         <v>1.37</v>
       </c>
     </row>
-    <row r="134" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A134" s="1">
         <v>44448</v>
       </c>
@@ -10255,7 +10254,7 @@
         <v>1.38</v>
       </c>
     </row>
-    <row r="135" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A135" s="1">
         <v>44448</v>
       </c>
@@ -10326,7 +10325,7 @@
         <v>1.34</v>
       </c>
     </row>
-    <row r="136" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A136" s="1">
         <v>44453</v>
       </c>
@@ -10397,7 +10396,7 @@
         <v>0.71</v>
       </c>
     </row>
-    <row r="137" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A137" s="1">
         <v>44453</v>
       </c>
@@ -10468,7 +10467,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="138" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A138" s="1">
         <v>44453</v>
       </c>
@@ -10539,7 +10538,7 @@
         <v>1.03</v>
       </c>
     </row>
-    <row r="139" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A139" s="1">
         <v>44453</v>
       </c>
@@ -10610,7 +10609,7 @@
         <v>1.02</v>
       </c>
     </row>
-    <row r="140" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A140" s="1">
         <v>44453</v>
       </c>
@@ -10681,7 +10680,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="141" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A141" s="1">
         <v>44453</v>
       </c>
@@ -10752,7 +10751,7 @@
         <v>1.02</v>
       </c>
     </row>
-    <row r="142" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A142" s="1">
         <v>44453</v>
       </c>
@@ -10823,7 +10822,7 @@
         <v>1.44</v>
       </c>
     </row>
-    <row r="143" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A143" s="1">
         <v>44453</v>
       </c>
@@ -10894,7 +10893,7 @@
         <v>1.33</v>
       </c>
     </row>
-    <row r="144" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A144" s="1">
         <v>44453</v>
       </c>
@@ -10965,7 +10964,7 @@
         <v>1.41</v>
       </c>
     </row>
-    <row r="145" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A145" s="1">
         <v>44453</v>
       </c>
@@ -11036,7 +11035,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="146" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A146" s="1">
         <v>44453</v>
       </c>
@@ -11107,7 +11106,7 @@
         <v>1.32</v>
       </c>
     </row>
-    <row r="147" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A147" s="1">
         <v>44453</v>
       </c>
@@ -11178,7 +11177,7 @@
         <v>2.11</v>
       </c>
     </row>
-    <row r="148" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A148" s="1">
         <v>44460</v>
       </c>
@@ -11246,7 +11245,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="149" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A149" s="1">
         <v>44460</v>
       </c>
@@ -11314,7 +11313,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="150" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A150" s="1">
         <v>44460</v>
       </c>
@@ -11382,7 +11381,7 @@
         <v>1.07</v>
       </c>
     </row>
-    <row r="151" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A151" s="1">
         <v>44460</v>
       </c>
@@ -11450,7 +11449,7 @@
         <v>1.07</v>
       </c>
     </row>
-    <row r="152" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A152" s="1">
         <v>44460</v>
       </c>
@@ -11518,7 +11517,7 @@
         <v>1.07</v>
       </c>
     </row>
-    <row r="153" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A153" s="1">
         <v>44460</v>
       </c>
@@ -11586,7 +11585,7 @@
         <v>1.42</v>
       </c>
     </row>
-    <row r="154" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A154" s="1">
         <v>44460</v>
       </c>
@@ -11654,7 +11653,7 @@
         <v>1.36</v>
       </c>
     </row>
-    <row r="155" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A155" s="1">
         <v>44460</v>
       </c>
@@ -11722,7 +11721,7 @@
         <v>1.38</v>
       </c>
     </row>
-    <row r="156" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A156" s="1">
         <v>44460</v>
       </c>
@@ -11790,7 +11789,7 @@
         <v>1.39</v>
       </c>
     </row>
-    <row r="157" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A157" s="1">
         <v>44463</v>
       </c>
@@ -11858,7 +11857,7 @@
         <v>1.24</v>
       </c>
     </row>
-    <row r="158" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A158" s="1">
         <v>44463</v>
       </c>
@@ -11926,7 +11925,7 @@
         <v>1.32</v>
       </c>
     </row>
-    <row r="159" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A159" s="1">
         <v>44467</v>
       </c>
@@ -11994,7 +11993,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="160" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A160" s="1">
         <v>44467</v>
       </c>
@@ -12062,7 +12061,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="161" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A161" s="1">
         <v>44467</v>
       </c>
@@ -12130,7 +12129,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="162" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A162" s="1">
         <v>44467</v>
       </c>
@@ -12198,7 +12197,7 @@
         <v>1.1200000000000001</v>
       </c>
     </row>
-    <row r="163" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A163" s="1">
         <v>44467</v>
       </c>
@@ -12266,7 +12265,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="164" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A164" s="1">
         <v>44467</v>
       </c>
@@ -12334,7 +12333,7 @@
         <v>1.39</v>
       </c>
     </row>
-    <row r="165" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A165" s="1">
         <v>44467</v>
       </c>
@@ -12402,7 +12401,7 @@
         <v>1.45</v>
       </c>
     </row>
-    <row r="166" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A166" s="1">
         <v>44467</v>
       </c>
@@ -12470,7 +12469,7 @@
         <v>1.46</v>
       </c>
     </row>
-    <row r="167" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A167" s="1">
         <v>44467</v>
       </c>
@@ -12538,7 +12537,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="168" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A168" s="1">
         <v>44468</v>
       </c>
@@ -12609,7 +12608,7 @@
         <v>1.1599999999999999</v>
       </c>
     </row>
-    <row r="169" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A169" s="1">
         <v>44468</v>
       </c>
@@ -12680,7 +12679,7 @@
         <v>2.78</v>
       </c>
     </row>
-    <row r="170" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A170" s="1">
         <v>44469</v>
       </c>
@@ -12751,7 +12750,7 @@
         <v>1.22</v>
       </c>
     </row>
-    <row r="171" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A171" s="1">
         <v>44469</v>
       </c>
@@ -12822,7 +12821,7 @@
         <v>1.85</v>
       </c>
     </row>
-    <row r="172" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A172" s="1">
         <v>44475</v>
       </c>
@@ -12890,7 +12889,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="173" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A173" s="1">
         <v>44475</v>
       </c>
@@ -12958,7 +12957,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="174" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A174" s="1">
         <v>44475</v>
       </c>
@@ -13026,7 +13025,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="175" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A175" s="1">
         <v>44475</v>
       </c>
@@ -13094,7 +13093,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="176" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A176" s="1">
         <v>44475</v>
       </c>
@@ -13162,7 +13161,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="177" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A177" s="1">
         <v>44475</v>
       </c>
@@ -13230,7 +13229,7 @@
         <v>1.1299999999999999</v>
       </c>
     </row>
-    <row r="178" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A178" s="1">
         <v>44475</v>
       </c>
@@ -13298,7 +13297,7 @@
         <v>1.1399999999999999</v>
       </c>
     </row>
-    <row r="179" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A179" s="1">
         <v>44475</v>
       </c>
@@ -13366,7 +13365,7 @@
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="180" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A180" s="1">
         <v>44475</v>
       </c>
@@ -13434,7 +13433,7 @@
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="181" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A181" s="1">
         <v>44481</v>
       </c>
@@ -13502,7 +13501,7 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="182" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A182" s="1">
         <v>44481</v>
       </c>
@@ -13570,7 +13569,7 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="183" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A183" s="1">
         <v>44481</v>
       </c>
@@ -13638,7 +13637,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="184" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A184" s="1">
         <v>44481</v>
       </c>
@@ -13706,7 +13705,7 @@
         <v>1.08</v>
       </c>
     </row>
-    <row r="185" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A185" s="1">
         <v>44481</v>
       </c>
@@ -13774,7 +13773,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="186" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A186" s="1">
         <v>44481</v>
       </c>
@@ -13842,7 +13841,7 @@
         <v>1.43</v>
       </c>
     </row>
-    <row r="187" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A187" s="1">
         <v>44481</v>
       </c>
@@ -13910,7 +13909,7 @@
         <v>1.48</v>
       </c>
     </row>
-    <row r="188" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A188" s="1">
         <v>44481</v>
       </c>
@@ -13978,7 +13977,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="189" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A189" s="1">
         <v>44481</v>
       </c>
@@ -14046,7 +14045,7 @@
         <v>1.48</v>
       </c>
     </row>
-    <row r="190" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A190" s="1">
         <v>44488</v>
       </c>
@@ -14114,7 +14113,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="191" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A191" s="1">
         <v>44488</v>
       </c>
@@ -14182,7 +14181,7 @@
         <v>1.03</v>
       </c>
     </row>
-    <row r="192" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A192" s="1">
         <v>44488</v>
       </c>
@@ -14250,7 +14249,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="193" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A193" s="1">
         <v>44488</v>
       </c>
@@ -14318,7 +14317,7 @@
         <v>1.03</v>
       </c>
     </row>
-    <row r="194" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A194" s="1">
         <v>44488</v>
       </c>
@@ -14386,7 +14385,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="195" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A195" s="1">
         <v>44488</v>
       </c>
@@ -14454,7 +14453,7 @@
         <v>1.38</v>
       </c>
     </row>
-    <row r="196" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A196" s="1">
         <v>44488</v>
       </c>
@@ -14522,7 +14521,7 @@
         <v>1.42</v>
       </c>
     </row>
-    <row r="197" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A197" s="1">
         <v>44488</v>
       </c>
@@ -14590,7 +14589,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="198" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A198" s="1">
         <v>44488</v>
       </c>
@@ -14658,7 +14657,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="199" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A199" s="1">
         <v>44491</v>
       </c>
@@ -14723,7 +14722,7 @@
         <v>1.23</v>
       </c>
     </row>
-    <row r="200" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A200" s="1">
         <v>44491</v>
       </c>
@@ -14788,7 +14787,7 @@
         <v>1.92</v>
       </c>
     </row>
-    <row r="201" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A201" s="1">
         <v>44494</v>
       </c>
@@ -14856,7 +14855,7 @@
         <v>1.17</v>
       </c>
     </row>
-    <row r="202" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A202" s="1">
         <v>44494</v>
       </c>
@@ -14924,7 +14923,7 @@
         <v>1.68</v>
       </c>
     </row>
-    <row r="203" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A203" s="1">
         <v>44495</v>
       </c>
@@ -14992,7 +14991,7 @@
         <v>1.41</v>
       </c>
     </row>
-    <row r="204" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A204" s="1">
         <v>44495</v>
       </c>
@@ -15060,7 +15059,7 @@
         <v>1.63</v>
       </c>
     </row>
-    <row r="205" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A205" s="1">
         <v>44496</v>
       </c>
@@ -15128,7 +15127,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="206" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A206" s="1">
         <v>44496</v>
       </c>
@@ -15196,7 +15195,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="207" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A207" s="1">
         <v>44496</v>
       </c>
@@ -15264,7 +15263,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="208" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A208" s="1">
         <v>44496</v>
       </c>
@@ -15332,7 +15331,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="209" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A209" s="1">
         <v>44496</v>
       </c>
@@ -15400,7 +15399,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="210" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A210" s="1">
         <v>44496</v>
       </c>
@@ -15468,7 +15467,7 @@
         <v>1.38</v>
       </c>
     </row>
-    <row r="211" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A211" s="1">
         <v>44496</v>
       </c>
@@ -15536,7 +15535,7 @@
         <v>1.39</v>
       </c>
     </row>
-    <row r="212" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A212" s="1">
         <v>44496</v>
       </c>
@@ -15604,7 +15603,7 @@
         <v>1.42</v>
       </c>
     </row>
-    <row r="213" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A213" s="1">
         <v>44496</v>
       </c>
@@ -15672,7 +15671,7 @@
         <v>1.45</v>
       </c>
     </row>
-    <row r="214" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A214" s="1">
         <v>44502</v>
       </c>
@@ -15740,7 +15739,7 @@
         <v>0.63</v>
       </c>
     </row>
-    <row r="215" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A215" s="1">
         <v>44502</v>
       </c>
@@ -15808,7 +15807,7 @@
         <v>1.19</v>
       </c>
     </row>
-    <row r="216" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A216" s="1">
         <v>44502</v>
       </c>
@@ -15876,7 +15875,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="217" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A217" s="1">
         <v>44502</v>
       </c>
@@ -15944,7 +15943,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="218" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A218" s="1">
         <v>44502</v>
       </c>
@@ -16012,7 +16011,7 @@
         <v>1.19</v>
       </c>
     </row>
-    <row r="219" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A219" s="1">
         <v>44502</v>
       </c>
@@ -16080,7 +16079,7 @@
         <v>1.58</v>
       </c>
     </row>
-    <row r="220" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A220" s="1">
         <v>44502</v>
       </c>
@@ -16148,7 +16147,7 @@
         <v>1.56</v>
       </c>
     </row>
-    <row r="221" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A221" s="1">
         <v>44502</v>
       </c>
@@ -16216,7 +16215,7 @@
         <v>1.56</v>
       </c>
     </row>
-    <row r="222" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A222" s="1">
         <v>44502</v>
       </c>
@@ -16284,7 +16283,7 @@
         <v>1.57</v>
       </c>
     </row>
-    <row r="223" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A223" s="1">
         <v>44502</v>
       </c>
@@ -16346,7 +16345,7 @@
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="224" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A224" s="1">
         <v>44508</v>
       </c>
@@ -16414,7 +16413,7 @@
         <v>0.63</v>
       </c>
     </row>
-    <row r="225" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A225" s="1">
         <v>44508</v>
       </c>
@@ -16482,7 +16481,7 @@
         <v>1.07</v>
       </c>
     </row>
-    <row r="226" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A226" s="1">
         <v>44508</v>
       </c>
@@ -16550,7 +16549,7 @@
         <v>1.1299999999999999</v>
       </c>
     </row>
-    <row r="227" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A227" s="1">
         <v>44508</v>
       </c>
@@ -16618,7 +16617,7 @@
         <v>1.1100000000000001</v>
       </c>
     </row>
-    <row r="228" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A228" s="1">
         <v>44508</v>
       </c>
@@ -16686,7 +16685,7 @@
         <v>1.1100000000000001</v>
       </c>
     </row>
-    <row r="229" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A229" s="1">
         <v>44508</v>
       </c>
@@ -16754,7 +16753,7 @@
         <v>1.43</v>
       </c>
     </row>
-    <row r="230" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A230" s="1">
         <v>44508</v>
       </c>
@@ -16822,7 +16821,7 @@
         <v>1.41</v>
       </c>
     </row>
-    <row r="231" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A231" s="1">
         <v>44508</v>
       </c>
@@ -16890,7 +16889,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="232" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A232" s="1">
         <v>44508</v>
       </c>
@@ -16958,7 +16957,7 @@
         <v>1.38</v>
       </c>
     </row>
-    <row r="233" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A233" s="1">
         <v>44508</v>
       </c>
@@ -17020,7 +17019,7 @@
         <v>1.26</v>
       </c>
     </row>
-    <row r="234" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A234" s="1">
         <v>44510</v>
       </c>
@@ -17088,7 +17087,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="235" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A235" s="1">
         <v>44510</v>
       </c>
@@ -17156,7 +17155,7 @@
         <v>1.1599999999999999</v>
       </c>
     </row>
-    <row r="236" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A236" s="1">
         <v>44510</v>
       </c>
@@ -17224,7 +17223,7 @@
         <v>1.1599999999999999</v>
       </c>
     </row>
-    <row r="237" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A237" s="1">
         <v>44510</v>
       </c>
@@ -17292,7 +17291,7 @@
         <v>1.1599999999999999</v>
       </c>
     </row>
-    <row r="238" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A238" s="1">
         <v>44510</v>
       </c>
@@ -17360,7 +17359,7 @@
         <v>1.1599999999999999</v>
       </c>
     </row>
-    <row r="239" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A239" s="1">
         <v>44510</v>
       </c>
@@ -17428,7 +17427,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="240" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A240" s="1">
         <v>44510</v>
       </c>
@@ -17496,7 +17495,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="241" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A241" s="1">
         <v>44510</v>
       </c>
@@ -17564,7 +17563,7 @@
         <v>1.52</v>
       </c>
     </row>
-    <row r="242" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A242" s="1">
         <v>44510</v>
       </c>
@@ -17632,7 +17631,7 @@
         <v>1.54</v>
       </c>
     </row>
-    <row r="243" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A243" s="1">
         <v>44512</v>
       </c>
@@ -17700,7 +17699,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="244" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A244" s="1">
         <v>44512</v>
       </c>
@@ -17768,7 +17767,7 @@
         <v>0.76</v>
       </c>
     </row>
-    <row r="245" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A245" s="1">
         <v>44516</v>
       </c>
@@ -17836,7 +17835,7 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="246" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A246" s="1">
         <v>44516</v>
       </c>
@@ -17904,7 +17903,7 @@
         <v>1.08</v>
       </c>
     </row>
-    <row r="247" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A247" s="1">
         <v>44516</v>
       </c>
@@ -17972,7 +17971,7 @@
         <v>1.08</v>
       </c>
     </row>
-    <row r="248" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A248" s="1">
         <v>44516</v>
       </c>
@@ -18040,7 +18039,7 @@
         <v>1.07</v>
       </c>
     </row>
-    <row r="249" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A249" s="1">
         <v>44516</v>
       </c>
@@ -18108,7 +18107,7 @@
         <v>1.08</v>
       </c>
     </row>
-    <row r="250" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A250" s="1">
         <v>44516</v>
       </c>
@@ -18176,7 +18175,7 @@
         <v>1.36</v>
       </c>
     </row>
-    <row r="251" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A251" s="1">
         <v>44516</v>
       </c>
@@ -18244,7 +18243,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="252" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A252" s="1">
         <v>44516</v>
       </c>
@@ -18312,7 +18311,7 @@
         <v>1.38</v>
       </c>
     </row>
-    <row r="253" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A253" s="1">
         <v>44516</v>
       </c>
@@ -18380,7 +18379,7 @@
         <v>1.37</v>
       </c>
     </row>
-    <row r="254" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A254" s="1">
         <v>44516</v>
       </c>
@@ -18442,7 +18441,7 @@
         <v>1.1299999999999999</v>
       </c>
     </row>
-    <row r="255" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A255" s="1">
         <v>44517</v>
       </c>
@@ -18510,7 +18509,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="256" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A256" s="1">
         <v>44517</v>
       </c>
@@ -18578,7 +18577,7 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="257" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A257" s="1">
         <v>44517</v>
       </c>
@@ -18646,7 +18645,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="258" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A258" s="1">
         <v>44518</v>
       </c>
@@ -18705,7 +18704,7 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="259" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A259" s="1">
         <v>44518</v>
       </c>
@@ -18764,7 +18763,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="260" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A260" s="1">
         <v>44518</v>
       </c>
@@ -18823,7 +18822,7 @@
         <v>1.07</v>
       </c>
     </row>
-    <row r="261" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A261" s="1">
         <v>44518</v>
       </c>
@@ -18882,7 +18881,7 @@
         <v>1.08</v>
       </c>
     </row>
-    <row r="262" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A262" s="1">
         <v>44518</v>
       </c>
@@ -18941,7 +18940,7 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="263" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A263" s="1">
         <v>44518</v>
       </c>
@@ -19000,7 +18999,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="264" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A264" s="1">
         <v>44518</v>
       </c>
@@ -19059,7 +19058,7 @@
         <v>1.32</v>
       </c>
     </row>
-    <row r="265" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A265" s="1">
         <v>44518</v>
       </c>
@@ -19118,7 +19117,7 @@
         <v>1.27</v>
       </c>
     </row>
-    <row r="266" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A266" s="1">
         <v>44518</v>
       </c>
@@ -19177,7 +19176,7 @@
         <v>1.29</v>
       </c>
     </row>
-    <row r="267" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A267" s="1">
         <v>44519</v>
       </c>
@@ -19245,7 +19244,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="268" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A268" s="1">
         <v>44519</v>
       </c>
@@ -19313,7 +19312,7 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="269" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A269" s="1">
         <v>44519</v>
       </c>
@@ -19381,7 +19380,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="270" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A270" s="1">
         <v>44522</v>
       </c>
@@ -19443,7 +19442,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="271" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A271" s="1">
         <v>44522</v>
       </c>
@@ -19505,7 +19504,7 @@
         <v>1.1399999999999999</v>
       </c>
     </row>
-    <row r="272" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A272" s="1">
         <v>44522</v>
       </c>
@@ -19567,7 +19566,7 @@
         <v>1.1399999999999999</v>
       </c>
     </row>
-    <row r="273" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A273" s="1">
         <v>44522</v>
       </c>
@@ -19629,7 +19628,7 @@
         <v>1.1399999999999999</v>
       </c>
     </row>
-    <row r="274" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A274" s="1">
         <v>44522</v>
       </c>
@@ -19691,7 +19690,7 @@
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="275" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A275" s="1">
         <v>44522</v>
       </c>
@@ -19753,7 +19752,7 @@
         <v>1.31</v>
       </c>
     </row>
-    <row r="276" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A276" s="1">
         <v>44522</v>
       </c>
@@ -19815,7 +19814,7 @@
         <v>1.31</v>
       </c>
     </row>
-    <row r="277" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A277" s="1">
         <v>44522</v>
       </c>
@@ -19877,7 +19876,7 @@
         <v>1.29</v>
       </c>
     </row>
-    <row r="278" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A278" s="1">
         <v>44522</v>
       </c>
@@ -19939,7 +19938,7 @@
         <v>1.29</v>
       </c>
     </row>
-    <row r="279" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A279" s="1">
         <v>44522</v>
       </c>
@@ -20001,7 +20000,7 @@
         <v>1.1399999999999999</v>
       </c>
     </row>
-    <row r="280" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A280" s="1">
         <v>44522</v>
       </c>
@@ -20063,7 +20062,7 @@
         <v>1.36</v>
       </c>
     </row>
-    <row r="281" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A281" s="1">
         <v>44523</v>
       </c>
@@ -20125,7 +20124,7 @@
         <v>1.33</v>
       </c>
     </row>
-    <row r="282" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A282" s="1">
         <v>44523</v>
       </c>

</xml_diff>